<commit_message>
updated suzie xml and excel sheet
</commit_message>
<xml_diff>
--- a/DividendLiberty/Suzie's IRA.xlsx
+++ b/DividendLiberty/Suzie's IRA.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steve Yi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steve Yi\Documents\GitHub\DividendLibertyCommercial\DividendLiberty\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Initial Buys" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="33">
   <si>
     <t>Symbols</t>
   </si>
@@ -117,6 +117,15 @@
   </si>
   <si>
     <t>2016 Dividends</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>AT&amp;T</t>
+  </si>
+  <si>
+    <t>Telecommunication</t>
   </si>
 </sst>
 </file>
@@ -552,8 +561,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AF40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W40" sqref="W40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,8 +650,12 @@
         <v>20</v>
       </c>
       <c r="U1" s="2"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="2"/>
+      <c r="V1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="W1" s="29" t="s">
+        <v>30</v>
+      </c>
       <c r="X1" s="2"/>
       <c r="Y1" s="3"/>
       <c r="Z1" s="2"/>
@@ -693,8 +706,12 @@
       <c r="T2" s="21">
         <v>840.48</v>
       </c>
-      <c r="V2" s="4"/>
-      <c r="W2" s="21"/>
+      <c r="V2" s="4">
+        <v>42629</v>
+      </c>
+      <c r="W2" s="21">
+        <v>1078.1099999999999</v>
+      </c>
       <c r="Y2" s="4"/>
       <c r="Z2" s="21"/>
       <c r="AB2" s="4"/>
@@ -702,10 +719,117 @@
       <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="W3" s="5"/>
       <c r="Z3" s="21"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="W4" s="5"/>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="W5" s="5"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="W6" s="5"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="W7" s="5"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="W8" s="5"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="W9" s="5"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="W10" s="5"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="W11" s="5"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="W12" s="5"/>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="W13" s="5"/>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="W14" s="5"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
+      <c r="W15" s="5"/>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="W16" s="5"/>
+    </row>
+    <row r="17" spans="23:23" x14ac:dyDescent="0.25">
+      <c r="W17" s="5"/>
+    </row>
+    <row r="18" spans="23:23" x14ac:dyDescent="0.25">
+      <c r="W18" s="5"/>
+    </row>
+    <row r="19" spans="23:23" x14ac:dyDescent="0.25">
+      <c r="W19" s="5"/>
+    </row>
+    <row r="20" spans="23:23" x14ac:dyDescent="0.25">
+      <c r="W20" s="5"/>
+    </row>
+    <row r="21" spans="23:23" x14ac:dyDescent="0.25">
+      <c r="W21" s="5"/>
+    </row>
+    <row r="22" spans="23:23" x14ac:dyDescent="0.25">
+      <c r="W22" s="5"/>
+    </row>
+    <row r="23" spans="23:23" x14ac:dyDescent="0.25">
+      <c r="W23" s="5"/>
+    </row>
+    <row r="24" spans="23:23" x14ac:dyDescent="0.25">
+      <c r="W24" s="5"/>
+    </row>
+    <row r="25" spans="23:23" x14ac:dyDescent="0.25">
+      <c r="W25" s="5"/>
+    </row>
+    <row r="26" spans="23:23" x14ac:dyDescent="0.25">
+      <c r="W26" s="5"/>
+    </row>
+    <row r="27" spans="23:23" x14ac:dyDescent="0.25">
+      <c r="W27" s="5"/>
+    </row>
+    <row r="28" spans="23:23" x14ac:dyDescent="0.25">
+      <c r="W28" s="5"/>
+    </row>
+    <row r="29" spans="23:23" x14ac:dyDescent="0.25">
+      <c r="W29" s="5"/>
+    </row>
+    <row r="30" spans="23:23" x14ac:dyDescent="0.25">
+      <c r="W30" s="5"/>
+    </row>
+    <row r="31" spans="23:23" x14ac:dyDescent="0.25">
+      <c r="W31" s="5"/>
+    </row>
+    <row r="32" spans="23:23" x14ac:dyDescent="0.25">
+      <c r="W32" s="5"/>
+    </row>
+    <row r="33" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="W33" s="5"/>
+    </row>
+    <row r="34" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="W34" s="5"/>
+    </row>
+    <row r="35" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="W35" s="5"/>
+    </row>
+    <row r="36" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="W36" s="5"/>
+    </row>
+    <row r="37" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="W37" s="5"/>
+    </row>
+    <row r="38" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="W38" s="5"/>
+    </row>
+    <row r="39" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="W39" s="5"/>
     </row>
     <row r="40" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B40" s="21">
@@ -736,7 +860,10 @@
         <f>SUM(T2:T39)</f>
         <v>840.48</v>
       </c>
-      <c r="W40" s="21"/>
+      <c r="W40" s="21">
+        <f>SUM(W2:W39)</f>
+        <v>1078.1099999999999</v>
+      </c>
       <c r="Z40" s="21"/>
       <c r="AC40" s="21"/>
     </row>
@@ -1353,17 +1480,17 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:V9"/>
+  <dimension ref="A1:V10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -1968,75 +2095,148 @@
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="20">
-        <f>SUM(G2:G8)</f>
+      <c r="A9" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="6">
+        <v>27</v>
+      </c>
+      <c r="E9" s="25">
+        <f t="shared" ref="E9" si="4">V9/D9</f>
+        <v>39.93</v>
+      </c>
+      <c r="F9" s="7">
+        <f>'Initial Buys'!W40</f>
+        <v>1078.1099999999999</v>
+      </c>
+      <c r="G9" s="19">
+        <v>0</v>
+      </c>
+      <c r="H9" s="28">
+        <v>0</v>
+      </c>
+      <c r="I9" s="26">
+        <v>0</v>
+      </c>
+      <c r="J9" s="28">
+        <v>0</v>
+      </c>
+      <c r="K9" s="26">
+        <v>0</v>
+      </c>
+      <c r="L9" s="28">
+        <v>0</v>
+      </c>
+      <c r="M9" s="26">
+        <v>0</v>
+      </c>
+      <c r="N9" s="28">
+        <v>0</v>
+      </c>
+      <c r="O9" s="26">
+        <v>0</v>
+      </c>
+      <c r="P9" s="28">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="26">
+        <v>0</v>
+      </c>
+      <c r="R9" s="28">
+        <v>0</v>
+      </c>
+      <c r="S9" s="26">
+        <v>0</v>
+      </c>
+      <c r="T9" s="19">
+        <f t="shared" ref="T9" si="5">SUM(H9:S9)</f>
+        <v>0</v>
+      </c>
+      <c r="U9" s="19">
+        <f t="shared" ref="U9" si="6">SUM(G9:S9)</f>
+        <v>0</v>
+      </c>
+      <c r="V9" s="17">
+        <f t="shared" ref="V9" si="7">SUM(F9, U9)</f>
+        <v>1078.1099999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="20">
+        <f>SUM(G2:G9)</f>
         <v>30.740000000000002</v>
       </c>
-      <c r="H9" s="27">
-        <f>SUM(H2:H8)</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="20">
-        <f t="shared" ref="I9:S9" si="4">SUM(I2:I8)</f>
-        <v>0</v>
-      </c>
-      <c r="J9" s="27">
-        <f t="shared" si="4"/>
+      <c r="H10" s="27">
+        <f>SUM(H2:H9)</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="20">
+        <f>SUM(I2:I9)</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="27">
+        <f>SUM(J2:J9)</f>
         <v>31.95</v>
       </c>
-      <c r="K9" s="20">
-        <f t="shared" si="4"/>
+      <c r="K10" s="20">
+        <f>SUM(K2:K9)</f>
         <v>7.66</v>
       </c>
-      <c r="L9" s="27">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M9" s="20">
-        <f t="shared" si="4"/>
+      <c r="L10" s="27">
+        <f>SUM(L2:L9)</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="20">
+        <f>SUM(M2:M9)</f>
         <v>39.5</v>
       </c>
-      <c r="N9" s="27">
-        <f t="shared" si="4"/>
+      <c r="N10" s="27">
+        <f>SUM(N2:N9)</f>
         <v>7.82</v>
       </c>
-      <c r="O9" s="20">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P9" s="27">
-        <f t="shared" si="4"/>
+      <c r="O10" s="20">
+        <f>SUM(O2:O9)</f>
+        <v>0</v>
+      </c>
+      <c r="P10" s="27">
+        <f>SUM(P2:P9)</f>
         <v>23.04</v>
       </c>
-      <c r="Q9" s="20">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="R9" s="27">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S9" s="20">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="T9" s="20">
-        <f>SUM(T2:T8)</f>
+      <c r="Q10" s="20">
+        <f>SUM(Q2:Q9)</f>
+        <v>0</v>
+      </c>
+      <c r="R10" s="27">
+        <f>SUM(R2:R9)</f>
+        <v>0</v>
+      </c>
+      <c r="S10" s="20">
+        <f>SUM(S2:S9)</f>
+        <v>0</v>
+      </c>
+      <c r="T10" s="20">
+        <f>SUM(T2:T9)</f>
         <v>109.97</v>
       </c>
-      <c r="U9" s="20">
-        <f>SUM(U2:U8)</f>
+      <c r="U10" s="20">
+        <f>SUM(U2:U9)</f>
         <v>140.70999999999998</v>
       </c>
-      <c r="V9" s="22">
-        <f>SUM(V2:V8)</f>
-        <v>5858.03</v>
+      <c r="V10" s="22">
+        <f>SUM(V2:V9)</f>
+        <v>6936.1399999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated suzie excel file.
</commit_message>
<xml_diff>
--- a/DividendLiberty/Suzie's IRA.xlsx
+++ b/DividendLiberty/Suzie's IRA.xlsx
@@ -596,7 +596,7 @@
   <dimension ref="A1:AF40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,8 +610,8 @@
     <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
@@ -753,6 +753,12 @@
       <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="J3" s="4">
+        <v>42696</v>
+      </c>
+      <c r="K3">
+        <v>703.29</v>
+      </c>
       <c r="V3" s="4">
         <v>42667</v>
       </c>
@@ -885,7 +891,7 @@
       </c>
       <c r="K40" s="21">
         <f>SUM(K2:K39)</f>
-        <v>859.32</v>
+        <v>1562.6100000000001</v>
       </c>
       <c r="N40" s="21">
         <f>SUM(N2:N39)</f>
@@ -1522,7 +1528,7 @@
   <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1848,15 +1854,15 @@
         <v>6</v>
       </c>
       <c r="D5" s="6">
-        <v>22.701000000000001</v>
+        <v>39.701000000000001</v>
       </c>
       <c r="E5" s="25">
         <f t="shared" si="0"/>
-        <v>39.202678296110307</v>
+        <v>40.130727185713205</v>
       </c>
       <c r="F5" s="7">
         <f>'Initial Buys'!K40</f>
-        <v>859.32</v>
+        <v>1562.6100000000001</v>
       </c>
       <c r="G5" s="19">
         <f>'2015'!S5</f>
@@ -1908,7 +1914,7 @@
       </c>
       <c r="V5" s="17">
         <f t="shared" si="3"/>
-        <v>889.94</v>
+        <v>1593.23</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -2275,7 +2281,7 @@
       </c>
       <c r="V10" s="22">
         <f t="shared" si="8"/>
-        <v>7620.83</v>
+        <v>8324.1200000000008</v>
       </c>
     </row>
   </sheetData>
@@ -2622,11 +2628,11 @@
       </c>
       <c r="E5" s="25">
         <f t="shared" si="0"/>
-        <v>39.52653786364646</v>
+        <v>70.763046857650451</v>
       </c>
       <c r="F5" s="7">
         <f>'Initial Buys'!K40</f>
-        <v>859.32</v>
+        <v>1562.6100000000001</v>
       </c>
       <c r="G5" s="19">
         <f>'2016'!U5</f>
@@ -2678,7 +2684,7 @@
       </c>
       <c r="V5" s="17">
         <f t="shared" si="3"/>
-        <v>889.94</v>
+        <v>1593.23</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -2972,7 +2978,7 @@
       </c>
       <c r="V9" s="22">
         <f>SUM(V2:V8)</f>
-        <v>5888.06</v>
+        <v>6591.3500000000013</v>
       </c>
     </row>
   </sheetData>

</xml_diff>